<commit_message>
translate, courses changed to replykeyboard
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -465,7 +465,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>sa</t>
+          <t>Sanjar Ibn Ravshan</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -480,7 +480,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>2023-01-08 10:11:16</t>
+          <t>2023-02-12 05:48:31</t>
         </is>
       </c>
     </row>

</xml_diff>